<commit_message>
i441--lse eit2 suite file update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/impl_00_LSE_engine.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/impl_00_LSE_engine.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{916B587F-92D3-430B-829A-C83C34B7C1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="402">
   <si>
     <t>CaseInfo</t>
   </si>
@@ -1252,16 +1253,34 @@
     <t>86</t>
   </si>
   <si>
-    <t>radiant=ng2_3</t>
-  </si>
-  <si>
-    <t>impl_00_LSE_engine_v2.00</t>
+    <t>UT_Case_updated/verilog_ut/260_1_state_machine_binary</t>
+  </si>
+  <si>
+    <t>UT_Case_updated/verilog_ut/260_2_state_machine_gray</t>
+  </si>
+  <si>
+    <t>UT_Case_updated/verilog_ut/260_3_state_machine_onehot</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>radiant=ng2022</t>
+  </si>
+  <si>
+    <t>impl_00_LSE_engine_v2.01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
@@ -2346,7 +2365,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2354,13 +2373,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47">
@@ -2420,7 +2439,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2456,22 +2475,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2501,22 +2511,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2531,13 +2535,13 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="24" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2558,22 +2562,22 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2694,19 +2698,19 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="49"/>
+    <cellStyle name="Hyperlink 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="41"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
-    <cellStyle name="Normal 3" xfId="44"/>
-    <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 6" xfId="43"/>
-    <cellStyle name="Normal 6 2" xfId="48"/>
-    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -2742,7 +2746,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4858,7 +4868,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4913,7 +4929,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4958,7 +4980,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5077,7 +5105,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5124,7 +5158,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5160,7 +5200,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{096177F5-3060-4E5D-96AA-950B4ADE6C37}" diskRevisions="1" revisionId="524" version="11">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F6019CB1-F56F-44AA-83F2-BCD7B91AD94B}" diskRevisions="1" revisionId="646" version="16">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5249,6 +5289,46 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{BC253C1D-3F5B-44A5-88E7-919A44D71DC9}" dateTime="2022-12-09T17:54:44" maxSheetId="5" userName="Jason Wang" r:id="rId12" minRId="525" maxRId="556">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FA61F358-98FC-49F1-8BF0-150FF1D3B951}" dateTime="2022-12-09T17:55:37" maxSheetId="5" userName="Jason Wang" r:id="rId13" minRId="557" maxRId="600">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0B056E9D-AD01-4FDE-A242-274889F2AB21}" dateTime="2022-12-09T17:55:43" maxSheetId="5" userName="Jason Wang" r:id="rId14" minRId="601">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BD47E64E-66A5-4A6F-BBFB-6F845E358D0B}" dateTime="2022-12-09T20:21:01" maxSheetId="5" userName="Jason Wang" r:id="rId15" minRId="602" maxRId="645">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F6019CB1-F56F-44AA-83F2-BCD7B91AD94B}" dateTime="2022-12-09T20:32:41" maxSheetId="5" userName="Jason Wang" r:id="rId16" minRId="646">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -5278,6 +5358,991 @@
     <nc r="B3" t="inlineStr">
       <is>
         <t>impl_00_LSE_engine_v2.00</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="525" sId="2" ref="A75:XFD75" action="insertRow"/>
+  <rrc rId="526" sId="2" ref="A75:XFD75" action="insertRow"/>
+  <rrc rId="527" sId="2" ref="A75:XFD75" action="insertRow"/>
+  <rcc rId="528" sId="2">
+    <nc r="E75" t="inlineStr">
+      <is>
+        <t>UT_Case_updated/verilog_ut/260_1_state_machine_binary</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="529" sId="2">
+    <nc r="E76" t="inlineStr">
+      <is>
+        <t>UT_Case_updated/verilog_ut/260_2_state_machine_gray</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="530" sId="2">
+    <nc r="E77" t="inlineStr">
+      <is>
+        <t>UT_Case_updated/verilog_ut/260_3_state_machine_onehot</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="531" sId="2">
+    <nc r="D75" t="inlineStr">
+      <is>
+        <t>JEDI</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="532" sId="2">
+    <nc r="D76" t="inlineStr">
+      <is>
+        <t>JEDI</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="533" sId="2">
+    <nc r="D77" t="inlineStr">
+      <is>
+        <t>JEDI</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="534" sId="2">
+    <nc r="A75" t="inlineStr">
+      <is>
+        <t>73</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="535" sId="2">
+    <nc r="A76" t="inlineStr">
+      <is>
+        <t>74</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="536" sId="2">
+    <nc r="A77" t="inlineStr">
+      <is>
+        <t>75</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="537" sId="2">
+    <oc r="A78" t="inlineStr">
+      <is>
+        <t>73</t>
+      </is>
+    </oc>
+    <nc r="A78" t="inlineStr">
+      <is>
+        <t>76</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="538" sId="2">
+    <oc r="A79" t="inlineStr">
+      <is>
+        <t>74</t>
+      </is>
+    </oc>
+    <nc r="A79" t="inlineStr">
+      <is>
+        <t>77</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="539" sId="2">
+    <oc r="A80" t="inlineStr">
+      <is>
+        <t>75</t>
+      </is>
+    </oc>
+    <nc r="A80" t="inlineStr">
+      <is>
+        <t>78</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="540" sId="2">
+    <oc r="A81" t="inlineStr">
+      <is>
+        <t>76</t>
+      </is>
+    </oc>
+    <nc r="A81" t="inlineStr">
+      <is>
+        <t>79</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="541" sId="2">
+    <oc r="A82" t="inlineStr">
+      <is>
+        <t>77</t>
+      </is>
+    </oc>
+    <nc r="A82" t="inlineStr">
+      <is>
+        <t>80</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="542" sId="2">
+    <oc r="A83" t="inlineStr">
+      <is>
+        <t>78</t>
+      </is>
+    </oc>
+    <nc r="A83" t="inlineStr">
+      <is>
+        <t>81</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="543" sId="2">
+    <oc r="A84" t="inlineStr">
+      <is>
+        <t>79</t>
+      </is>
+    </oc>
+    <nc r="A84" t="inlineStr">
+      <is>
+        <t>82</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="544" sId="2">
+    <oc r="A85" t="inlineStr">
+      <is>
+        <t>80</t>
+      </is>
+    </oc>
+    <nc r="A85" t="inlineStr">
+      <is>
+        <t>83</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="545" sId="2">
+    <oc r="A86" t="inlineStr">
+      <is>
+        <t>81</t>
+      </is>
+    </oc>
+    <nc r="A86" t="inlineStr">
+      <is>
+        <t>84</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="546" sId="2">
+    <oc r="A87" t="inlineStr">
+      <is>
+        <t>82</t>
+      </is>
+    </oc>
+    <nc r="A87" t="inlineStr">
+      <is>
+        <t>85</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="547" sId="2">
+    <oc r="A88" t="inlineStr">
+      <is>
+        <t>83</t>
+      </is>
+    </oc>
+    <nc r="A88" t="inlineStr">
+      <is>
+        <t>86</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="548" sId="2">
+    <oc r="A89" t="inlineStr">
+      <is>
+        <t>84</t>
+      </is>
+    </oc>
+    <nc r="A89" t="inlineStr">
+      <is>
+        <t>87</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="549" sId="2">
+    <oc r="A90" t="inlineStr">
+      <is>
+        <t>85</t>
+      </is>
+    </oc>
+    <nc r="A90" t="inlineStr">
+      <is>
+        <t>88</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="550" sId="2">
+    <oc r="A91" t="inlineStr">
+      <is>
+        <t>86</t>
+      </is>
+    </oc>
+    <nc r="A91" t="inlineStr">
+      <is>
+        <t>89</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="551" sId="2">
+    <nc r="O75" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LIFCL-40-7BG400I</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="552" sId="2">
+    <nc r="S75" t="inlineStr">
+      <is>
+        <t>synthesis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="553" sId="2">
+    <nc r="O76" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LIFCL-40-7BG400I</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="554" sId="2">
+    <nc r="S76" t="inlineStr">
+      <is>
+        <t>synthesis</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="555" sId="2">
+    <nc r="O77" t="inlineStr">
+      <is>
+        <t>cmd = --devkit=LIFCL-40-7BG400I</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="556" sId="2">
+    <nc r="S77" t="inlineStr">
+      <is>
+        <t>synthesis</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="557" sId="2">
+    <nc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="558" sId="2">
+    <nc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="559" sId="2">
+    <nc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="560" sId="2">
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="561" sId="2">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="562" sId="2">
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="563" sId="2">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="564" sId="2">
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="565" sId="2">
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="566" sId="2">
+    <nc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="567" sId="2">
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="568" sId="2">
+    <nc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="569" sId="2">
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="570" sId="2">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="571" sId="2">
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="572" sId="2">
+    <nc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="573" sId="2">
+    <nc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="574" sId="2">
+    <nc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="575" sId="2">
+    <nc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="576" sId="2">
+    <nc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="577" sId="2">
+    <nc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="578" sId="2">
+    <nc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="579" sId="2">
+    <nc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="580" sId="2">
+    <nc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="581" sId="2">
+    <nc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="582" sId="2">
+    <nc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="583" sId="2">
+    <nc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="584" sId="2">
+    <nc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="585" sId="2">
+    <nc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="586" sId="2">
+    <nc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="587" sId="2">
+    <nc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="588" sId="2">
+    <nc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="589" sId="2">
+    <nc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="590" sId="2">
+    <nc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="591" sId="2">
+    <nc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="592" sId="2">
+    <nc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="593" sId="2">
+    <nc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="594" sId="2">
+    <nc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="595" sId="2">
+    <nc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="596" sId="2">
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="597" sId="2">
+    <nc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="598" sId="2">
+    <nc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="599" sId="2">
+    <nc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="600" sId="2">
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="601" sId="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_3</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2022</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="602" sId="2">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B3"/>
+  </rcc>
+  <rcc rId="603" sId="2">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B4"/>
+  </rcc>
+  <rcc rId="604" sId="2">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B5"/>
+  </rcc>
+  <rcc rId="605" sId="2">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B6"/>
+  </rcc>
+  <rcc rId="606" sId="2">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B7"/>
+  </rcc>
+  <rcc rId="607" sId="2">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B8"/>
+  </rcc>
+  <rcc rId="608" sId="2">
+    <oc r="B9" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B9"/>
+  </rcc>
+  <rcc rId="609" sId="2">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B10"/>
+  </rcc>
+  <rcc rId="610" sId="2">
+    <oc r="B11" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B11"/>
+  </rcc>
+  <rcc rId="611" sId="2">
+    <oc r="B12" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B12"/>
+  </rcc>
+  <rcc rId="612" sId="2">
+    <oc r="B13" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B13"/>
+  </rcc>
+  <rcc rId="613" sId="2">
+    <oc r="B14" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B14"/>
+  </rcc>
+  <rcc rId="614" sId="2">
+    <oc r="B15" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B15"/>
+  </rcc>
+  <rcc rId="615" sId="2">
+    <oc r="B16" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B16"/>
+  </rcc>
+  <rcc rId="616" sId="2">
+    <oc r="B17" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B17"/>
+  </rcc>
+  <rcc rId="617" sId="2">
+    <oc r="B18" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B18"/>
+  </rcc>
+  <rcc rId="618" sId="2">
+    <oc r="B19" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B19"/>
+  </rcc>
+  <rcc rId="619" sId="2">
+    <oc r="B20" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B20"/>
+  </rcc>
+  <rcc rId="620" sId="2">
+    <oc r="B21" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B21"/>
+  </rcc>
+  <rcc rId="621" sId="2">
+    <oc r="B22" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B22"/>
+  </rcc>
+  <rcc rId="622" sId="2">
+    <oc r="B23" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B23"/>
+  </rcc>
+  <rcc rId="623" sId="2">
+    <oc r="B24" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B24"/>
+  </rcc>
+  <rcc rId="624" sId="2">
+    <oc r="B25" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B25"/>
+  </rcc>
+  <rcc rId="625" sId="2">
+    <oc r="B26" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B26"/>
+  </rcc>
+  <rcc rId="626" sId="2">
+    <oc r="B27" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B27"/>
+  </rcc>
+  <rcc rId="627" sId="2">
+    <oc r="B28" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B28"/>
+  </rcc>
+  <rcc rId="628" sId="2">
+    <oc r="B29" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B29"/>
+  </rcc>
+  <rcc rId="629" sId="2">
+    <oc r="B30" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B30"/>
+  </rcc>
+  <rcc rId="630" sId="2">
+    <oc r="B31" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B31"/>
+  </rcc>
+  <rcc rId="631" sId="2">
+    <oc r="B32" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B32"/>
+  </rcc>
+  <rcc rId="632" sId="2">
+    <oc r="B33" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B33"/>
+  </rcc>
+  <rcc rId="633" sId="2">
+    <oc r="B34" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B34"/>
+  </rcc>
+  <rcc rId="634" sId="2">
+    <oc r="B35" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B35"/>
+  </rcc>
+  <rcc rId="635" sId="2">
+    <oc r="B36" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B36"/>
+  </rcc>
+  <rcc rId="636" sId="2">
+    <oc r="B37" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B37"/>
+  </rcc>
+  <rcc rId="637" sId="2">
+    <oc r="B38" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B38"/>
+  </rcc>
+  <rcc rId="638" sId="2">
+    <oc r="B39" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B39"/>
+  </rcc>
+  <rcc rId="639" sId="2">
+    <oc r="B40" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B40"/>
+  </rcc>
+  <rcc rId="640" sId="2">
+    <oc r="B41" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B41"/>
+  </rcc>
+  <rcc rId="641" sId="2">
+    <oc r="B42" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B42"/>
+  </rcc>
+  <rcc rId="642" sId="2">
+    <oc r="B43" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B43"/>
+  </rcc>
+  <rcc rId="643" sId="2">
+    <oc r="B44" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B44"/>
+  </rcc>
+  <rcc rId="644" sId="2">
+    <oc r="B45" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B45"/>
+  </rcc>
+  <rcc rId="645" sId="2">
+    <oc r="B46" t="inlineStr">
+      <is>
+        <t>YES</t>
+      </is>
+    </oc>
+    <nc r="B46"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="646" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>impl_00_LSE_engine_v2.00</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>impl_00_LSE_engine_v2.01</t>
       </is>
     </nc>
   </rcc>
@@ -9121,6 +10186,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9156,6 +10238,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9331,14 +10430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="2" customWidth="1"/>
@@ -9366,7 +10465,7 @@
         <v>255</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -9400,7 +10499,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -9449,83 +10548,83 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AD91"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
+      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="2" customWidth="1"/>
     <col min="8" max="8" width="37" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="30.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="13" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" style="2" customWidth="1"/>
     <col min="21" max="21" width="11" style="2" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" style="2" customWidth="1"/>
     <col min="23" max="28" width="9" style="2"/>
-    <col min="29" max="29" width="10.140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="10.109375" style="2" customWidth="1"/>
     <col min="30" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:30" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-    </row>
-    <row r="2" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+    </row>
+    <row r="2" spans="1:30" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -9617,7 +10716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.75" thickTop="1">
+    <row r="3" spans="1:30" ht="15" thickTop="1">
       <c r="A3" s="2" t="s">
         <v>260</v>
       </c>
@@ -10849,7 +11948,7 @@
         <v>351</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>323</v>
+        <v>394</v>
       </c>
       <c r="O75" s="2" t="s">
         <v>352</v>
@@ -10866,7 +11965,7 @@
         <v>351</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>325</v>
+        <v>395</v>
       </c>
       <c r="O76" s="2" t="s">
         <v>352</v>
@@ -10883,7 +11982,7 @@
         <v>351</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>327</v>
+        <v>396</v>
       </c>
       <c r="O77" s="2" t="s">
         <v>352</v>
@@ -10900,7 +11999,7 @@
         <v>351</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="O78" s="2" t="s">
         <v>352</v>
@@ -10917,7 +12016,7 @@
         <v>351</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="O79" s="2" t="s">
         <v>352</v>
@@ -10934,7 +12033,7 @@
         <v>351</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="O80" s="2" t="s">
         <v>352</v>
@@ -10951,7 +12050,7 @@
         <v>351</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="O81" s="2" t="s">
         <v>352</v>
@@ -10968,7 +12067,7 @@
         <v>351</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>352</v>
@@ -10985,7 +12084,7 @@
         <v>351</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="O83" s="2" t="s">
         <v>352</v>
@@ -11002,7 +12101,7 @@
         <v>351</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>352</v>
@@ -11019,7 +12118,7 @@
         <v>351</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>352</v>
@@ -11036,7 +12135,7 @@
         <v>351</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="O86" s="2" t="s">
         <v>352</v>
@@ -11053,7 +12152,7 @@
         <v>351</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>352</v>
@@ -11070,7 +12169,7 @@
         <v>351</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="O88" s="2" t="s">
         <v>352</v>
@@ -11079,37 +12178,88 @@
         <v>264</v>
       </c>
     </row>
+    <row r="89" spans="1:19">
+      <c r="A89" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="O89" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
+      <c r="A90" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="O90" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="S90" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
+      <c r="A91" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="O91" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AD2"/>
+  <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{EF0F864A-F4B6-4709-8464-9BCA64517901}"/>
     </customSheetView>
     <customSheetView guid="{0278B0C9-EFE0-4CCF-A7DD-30F52F97656D}" scale="40" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="AH69" sqref="AH69"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{23A2521D-8A41-4664-9C0D-B198A8619A1B}"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{B4AB0BFD-F7A2-4A44-94B4-C91F8C036A1B}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{5BEF0A4F-A3B7-4FEE-8379-0C9E97FBE5ED}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -11118,10 +12268,10 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 W1:AA1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 W1:AA1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:V1 A1 C1:E1 G1:H1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:V1 A1 C1:E1 G1:H1" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$F$31:$J$31</formula1>
     </dataValidation>
   </dataValidations>
@@ -11130,49 +12280,49 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>description!$F$140:$H$140</xm:f>
           </x14:formula1>
           <xm:sqref>AB1:AB1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>description!$F$141:$H$141</xm:f>
           </x14:formula1>
           <xm:sqref>AC1:AC1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>description!$F$121:$K$121</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>description!$F$123:$H$123</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>description!$E$113:$F$113</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>description!$F$117:$H$117</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>description!$F$120:$K$120</xm:f>
           </x14:formula1>
@@ -11185,25 +12335,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="19" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="15" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="32" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -11226,7 +12376,7 @@
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="108" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="109" spans="1:14" ht="12.75" customHeight="1"/>
-    <row r="110" spans="1:14" ht="15.75" thickBot="1">
+    <row r="110" spans="1:14" ht="15" thickBot="1">
       <c r="A110" s="6" t="s">
         <v>71</v>
       </c>
@@ -11234,7 +12384,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15.75" thickBot="1">
+    <row r="111" spans="1:14" ht="15" thickBot="1">
       <c r="A111" s="9" t="s">
         <v>73</v>
       </c>
@@ -11250,17 +12400,17 @@
       <c r="E111" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F111" s="104" t="s">
+      <c r="F111" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="G111" s="105"/>
-      <c r="H111" s="105"/>
-      <c r="I111" s="105"/>
-      <c r="J111" s="105"/>
-      <c r="K111" s="105"/>
-      <c r="L111" s="105"/>
-      <c r="M111" s="105"/>
-      <c r="N111" s="106"/>
+      <c r="G111" s="100"/>
+      <c r="H111" s="100"/>
+      <c r="I111" s="100"/>
+      <c r="J111" s="100"/>
+      <c r="K111" s="100"/>
+      <c r="L111" s="100"/>
+      <c r="M111" s="100"/>
+      <c r="N111" s="101"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -12062,7 +13212,7 @@
       <c r="M141" s="18"/>
       <c r="N141" s="19"/>
     </row>
-    <row r="142" spans="1:14" ht="15.75" thickBot="1">
+    <row r="142" spans="1:14" ht="15" thickBot="1">
       <c r="A142" s="20" t="s">
         <v>112</v>
       </c>
@@ -12086,7 +13236,7 @@
       <c r="M142" s="21"/>
       <c r="N142" s="22"/>
     </row>
-    <row r="145" spans="1:8" ht="15.75" thickBot="1">
+    <row r="145" spans="1:8" ht="15" thickBot="1">
       <c r="A145" s="6" t="s">
         <v>113</v>
       </c>
@@ -12124,7 +13274,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="89" t="s">
+      <c r="B147" s="84" t="s">
         <v>0</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -12150,7 +13300,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="90"/>
+      <c r="B148" s="85"/>
       <c r="C148" s="28" t="s">
         <v>126</v>
       </c>
@@ -12172,7 +13322,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="90"/>
+      <c r="B149" s="85"/>
       <c r="C149" s="28" t="s">
         <v>6</v>
       </c>
@@ -12192,7 +13342,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="90"/>
+      <c r="B150" s="85"/>
       <c r="C150" s="28" t="s">
         <v>128</v>
       </c>
@@ -12216,7 +13366,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="90"/>
+      <c r="B151" s="85"/>
       <c r="C151" s="27" t="s">
         <v>130</v>
       </c>
@@ -12240,7 +13390,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="90"/>
+      <c r="B152" s="85"/>
       <c r="C152" s="27" t="s">
         <v>134</v>
       </c>
@@ -12264,7 +13414,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="90"/>
+      <c r="B153" s="85"/>
       <c r="C153" s="28" t="s">
         <v>137</v>
       </c>
@@ -12286,7 +13436,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="90"/>
+      <c r="B154" s="85"/>
       <c r="C154" s="27" t="s">
         <v>138</v>
       </c>
@@ -12310,7 +13460,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="90"/>
+      <c r="B155" s="85"/>
       <c r="C155" s="27" t="s">
         <v>139</v>
       </c>
@@ -12334,7 +13484,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="90"/>
+      <c r="B156" s="85"/>
       <c r="C156" s="28" t="s">
         <v>140</v>
       </c>
@@ -12358,7 +13508,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="90"/>
+      <c r="B157" s="85"/>
       <c r="C157" s="28" t="s">
         <v>141</v>
       </c>
@@ -12382,7 +13532,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="90"/>
+      <c r="B158" s="85"/>
       <c r="C158" s="28" t="s">
         <v>143</v>
       </c>
@@ -12404,7 +13554,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="84"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="28" t="s">
         <v>52</v>
       </c>
@@ -12428,7 +13578,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="80" t="s">
+      <c r="B160" s="75" t="s">
         <v>1</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -12454,7 +13604,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="79"/>
+      <c r="B161" s="74"/>
       <c r="C161" s="28" t="s">
         <v>151</v>
       </c>
@@ -12478,7 +13628,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="89" t="s">
+      <c r="B162" s="84" t="s">
         <v>2</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -12502,7 +13652,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="107"/>
+      <c r="B163" s="102"/>
       <c r="C163" s="27" t="s">
         <v>155</v>
       </c>
@@ -12524,7 +13674,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="84"/>
+      <c r="B164" s="79"/>
       <c r="C164" s="27" t="s">
         <v>157</v>
       </c>
@@ -12544,7 +13694,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="80" t="s">
+      <c r="B165" s="75" t="s">
         <v>3</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -12568,7 +13718,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="79"/>
+      <c r="B166" s="74"/>
       <c r="C166" s="28" t="s">
         <v>162</v>
       </c>
@@ -12588,7 +13738,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="79"/>
+      <c r="B167" s="74"/>
       <c r="C167" s="28" t="s">
         <v>163</v>
       </c>
@@ -12608,7 +13758,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="79"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="28" t="s">
         <v>164</v>
       </c>
@@ -12628,7 +13778,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="79"/>
+      <c r="B169" s="74"/>
       <c r="C169" s="28" t="s">
         <v>165</v>
       </c>
@@ -12648,7 +13798,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="79"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="28" t="s">
         <v>166</v>
       </c>
@@ -12668,7 +13818,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="79"/>
+      <c r="B171" s="74"/>
       <c r="C171" s="28" t="s">
         <v>167</v>
       </c>
@@ -12688,7 +13838,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="79"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="28" t="s">
         <v>37</v>
       </c>
@@ -12704,11 +13854,11 @@
       </c>
       <c r="H172" s="16"/>
     </row>
-    <row r="173" spans="1:8" ht="90">
+    <row r="173" spans="1:8" ht="86.4">
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="80" t="s">
+      <c r="B173" s="75" t="s">
         <v>4</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -12732,7 +13882,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="79"/>
+      <c r="B174" s="74"/>
       <c r="C174" s="27" t="s">
         <v>171</v>
       </c>
@@ -12754,7 +13904,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="79"/>
+      <c r="B175" s="74"/>
       <c r="C175" s="28" t="s">
         <v>174</v>
       </c>
@@ -12776,7 +13926,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="89" t="s">
+      <c r="B176" s="84" t="s">
         <v>5</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -12798,11 +13948,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="15.75" thickBot="1">
+    <row r="177" spans="1:8" ht="15" thickBot="1">
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="90"/>
+      <c r="B177" s="85"/>
       <c r="C177" s="32" t="s">
         <v>179</v>
       </c>
@@ -12826,7 +13976,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="91" t="s">
+      <c r="B178" s="86" t="s">
         <v>181</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -12850,7 +14000,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="92"/>
+      <c r="B179" s="87"/>
       <c r="C179" s="27" t="s">
         <v>185</v>
       </c>
@@ -12872,7 +14022,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="93"/>
+      <c r="B180" s="88"/>
       <c r="C180" s="34" t="s">
         <v>188</v>
       </c>
@@ -12894,7 +14044,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="93"/>
+      <c r="B181" s="88"/>
       <c r="C181" s="34" t="s">
         <v>189</v>
       </c>
@@ -12916,17 +14066,17 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="93"/>
+      <c r="B182" s="88"/>
       <c r="C182" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="D182" s="42" t="s">
+      <c r="D182" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E182" s="42" t="s">
+      <c r="E182" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F182" s="42"/>
+      <c r="F182" s="32"/>
       <c r="G182" s="34" t="s">
         <v>250</v>
       </c>
@@ -12936,15 +14086,15 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="93"/>
+      <c r="B183" s="88"/>
       <c r="C183" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="D183" s="42" t="s">
+      <c r="D183" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E183" s="42"/>
-      <c r="F183" s="42" t="s">
+      <c r="E183" s="32"/>
+      <c r="F183" s="32" t="s">
         <v>245</v>
       </c>
       <c r="G183" s="34" t="s">
@@ -12954,11 +14104,11 @@
         <v>247</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="15.75" thickBot="1">
+    <row r="184" spans="1:8" ht="15" thickBot="1">
       <c r="A184" s="35">
         <v>38</v>
       </c>
-      <c r="B184" s="88"/>
+      <c r="B184" s="83"/>
       <c r="C184" s="36" t="s">
         <v>248</v>
       </c>
@@ -12985,7 +14135,7 @@
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="B186" s="37" t="s">
+      <c r="B186" s="6" t="s">
         <v>195</v>
       </c>
     </row>
@@ -12994,7 +14144,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15.75" thickBot="1">
+    <row r="197" spans="1:7" ht="15" thickBot="1">
       <c r="A197" s="6" t="s">
         <v>197</v>
       </c>
@@ -13006,280 +14156,280 @@
       <c r="A198" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B198" s="38" t="s">
+      <c r="B198" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="C198" s="94" t="s">
+      <c r="C198" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="D198" s="94"/>
-      <c r="E198" s="94"/>
-      <c r="F198" s="39" t="s">
+      <c r="D198" s="89"/>
+      <c r="E198" s="89"/>
+      <c r="F198" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="G198" s="40" t="s">
+      <c r="G198" s="38" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="77" t="s">
+      <c r="A199" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="B199" s="79" t="s">
+      <c r="B199" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="C199" s="96" t="s">
+      <c r="C199" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="D199" s="97"/>
-      <c r="E199" s="97"/>
+      <c r="D199" s="92"/>
+      <c r="E199" s="92"/>
       <c r="F199" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G199" s="41" t="s">
+      <c r="G199" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="77"/>
-      <c r="B200" s="95"/>
-      <c r="C200" s="98" t="s">
+      <c r="A200" s="72"/>
+      <c r="B200" s="90"/>
+      <c r="C200" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="D200" s="99"/>
-      <c r="E200" s="99"/>
+      <c r="D200" s="94"/>
+      <c r="E200" s="94"/>
       <c r="F200" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="G200" s="43" t="s">
+      <c r="G200" s="40" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="77"/>
-      <c r="B201" s="79" t="s">
+      <c r="A201" s="72"/>
+      <c r="B201" s="74" t="s">
         <v>206</v>
       </c>
-      <c r="C201" s="100" t="s">
+      <c r="C201" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="D201" s="100"/>
-      <c r="E201" s="100"/>
+      <c r="D201" s="95"/>
+      <c r="E201" s="95"/>
       <c r="F201" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G201" s="41" t="s">
+      <c r="G201" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="77"/>
-      <c r="B202" s="79"/>
-      <c r="C202" s="98" t="s">
+      <c r="A202" s="72"/>
+      <c r="B202" s="74"/>
+      <c r="C202" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="D202" s="98"/>
-      <c r="E202" s="98"/>
+      <c r="D202" s="93"/>
+      <c r="E202" s="93"/>
       <c r="F202" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G202" s="41" t="s">
+      <c r="G202" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="77"/>
-      <c r="B203" s="95" t="s">
+      <c r="A203" s="72"/>
+      <c r="B203" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="C203" s="101" t="s">
+      <c r="C203" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="D203" s="102"/>
-      <c r="E203" s="103"/>
+      <c r="D203" s="97"/>
+      <c r="E203" s="98"/>
       <c r="F203" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G203" s="41" t="s">
+      <c r="G203" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="77"/>
-      <c r="B204" s="84"/>
-      <c r="C204" s="101" t="s">
+      <c r="A204" s="72"/>
+      <c r="B204" s="79"/>
+      <c r="C204" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="D204" s="102"/>
-      <c r="E204" s="103"/>
+      <c r="D204" s="97"/>
+      <c r="E204" s="98"/>
       <c r="F204" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G204" s="41" t="s">
+      <c r="G204" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="77"/>
-      <c r="B205" s="79" t="s">
+      <c r="A205" s="72"/>
+      <c r="B205" s="74" t="s">
         <v>209</v>
       </c>
-      <c r="C205" s="100" t="s">
+      <c r="C205" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="D205" s="100"/>
-      <c r="E205" s="100"/>
+      <c r="D205" s="95"/>
+      <c r="E205" s="95"/>
       <c r="F205" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G205" s="41" t="s">
+      <c r="G205" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="77"/>
-      <c r="B206" s="79"/>
-      <c r="C206" s="100" t="s">
+      <c r="A206" s="72"/>
+      <c r="B206" s="74"/>
+      <c r="C206" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="D206" s="100"/>
-      <c r="E206" s="100"/>
+      <c r="D206" s="95"/>
+      <c r="E206" s="95"/>
       <c r="F206" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G206" s="41" t="s">
+      <c r="G206" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="77" t="s">
+      <c r="A207" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="B207" s="79" t="s">
+      <c r="B207" s="74" t="s">
         <v>212</v>
       </c>
-      <c r="C207" s="80" t="s">
+      <c r="C207" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="D207" s="79"/>
-      <c r="E207" s="79"/>
+      <c r="D207" s="74"/>
+      <c r="E207" s="74"/>
       <c r="F207" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G207" s="41" t="s">
+      <c r="G207" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="77"/>
-      <c r="B208" s="79"/>
-      <c r="C208" s="79" t="s">
+      <c r="A208" s="72"/>
+      <c r="B208" s="74"/>
+      <c r="C208" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="D208" s="79"/>
-      <c r="E208" s="79"/>
+      <c r="D208" s="74"/>
+      <c r="E208" s="74"/>
       <c r="F208" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G208" s="41" t="s">
+      <c r="G208" s="39" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="77"/>
-      <c r="B209" s="79" t="s">
+      <c r="A209" s="72"/>
+      <c r="B209" s="74" t="s">
         <v>214</v>
       </c>
-      <c r="C209" s="79" t="s">
+      <c r="C209" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D209" s="79"/>
-      <c r="E209" s="79"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="74"/>
       <c r="F209" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G209" s="41" t="s">
+      <c r="G209" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="77"/>
-      <c r="B210" s="79"/>
-      <c r="C210" s="79" t="s">
+      <c r="A210" s="72"/>
+      <c r="B210" s="74"/>
+      <c r="C210" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="D210" s="79"/>
-      <c r="E210" s="79"/>
+      <c r="D210" s="74"/>
+      <c r="E210" s="74"/>
       <c r="F210" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G210" s="41" t="s">
+      <c r="G210" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="77" t="s">
+      <c r="A211" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="B211" s="79" t="s">
+      <c r="B211" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="C211" s="80" t="s">
+      <c r="C211" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="D211" s="79"/>
-      <c r="E211" s="79"/>
+      <c r="D211" s="74"/>
+      <c r="E211" s="74"/>
       <c r="F211" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G211" s="41" t="s">
+      <c r="G211" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="77"/>
-      <c r="B212" s="79"/>
-      <c r="C212" s="79" t="s">
+      <c r="A212" s="72"/>
+      <c r="B212" s="74"/>
+      <c r="C212" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D212" s="79"/>
-      <c r="E212" s="79"/>
+      <c r="D212" s="74"/>
+      <c r="E212" s="74"/>
       <c r="F212" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="G212" s="41" t="s">
+      <c r="G212" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="77"/>
-      <c r="B213" s="79" t="s">
+      <c r="A213" s="72"/>
+      <c r="B213" s="74" t="s">
         <v>217</v>
       </c>
-      <c r="C213" s="80" t="s">
+      <c r="C213" s="75" t="s">
         <v>218</v>
       </c>
-      <c r="D213" s="79"/>
-      <c r="E213" s="79"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="74"/>
       <c r="F213" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G213" s="41" t="s">
+      <c r="G213" s="39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="78"/>
-      <c r="B214" s="81"/>
-      <c r="C214" s="81" t="s">
+    <row r="214" spans="1:7" ht="15" thickBot="1">
+      <c r="A214" s="73"/>
+      <c r="B214" s="76"/>
+      <c r="C214" s="76" t="s">
         <v>219</v>
       </c>
-      <c r="D214" s="81"/>
-      <c r="E214" s="81"/>
+      <c r="D214" s="76"/>
+      <c r="E214" s="76"/>
       <c r="F214" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="G214" s="44" t="s">
+      <c r="G214" s="41" t="s">
         <v>59</v>
       </c>
     </row>
@@ -13287,60 +14437,43 @@
       <c r="A215" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C215" s="37"/>
-      <c r="D215" s="37"/>
-      <c r="E215" s="37"/>
-      <c r="F215" s="37"/>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="C216" s="37"/>
-      <c r="D216" s="37"/>
-      <c r="E216" s="37"/>
-    </row>
-    <row r="217" spans="1:7">
-      <c r="C217" s="37"/>
-      <c r="D217" s="37"/>
-      <c r="E217" s="37"/>
-    </row>
-    <row r="218" spans="1:7" ht="15.75" thickBot="1">
+    </row>
+    <row r="218" spans="1:7" ht="15" thickBot="1">
       <c r="A218" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C218" s="37"/>
-      <c r="D218" s="37"/>
-      <c r="E218" s="37"/>
-    </row>
-    <row r="219" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A219" s="45" t="s">
+    </row>
+    <row r="219" spans="1:7" ht="15" thickBot="1">
+      <c r="A219" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="B219" s="82" t="s">
+      <c r="B219" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="C219" s="82"/>
-      <c r="D219" s="82"/>
-      <c r="E219" s="82"/>
-      <c r="F219" s="46" t="s">
+      <c r="C219" s="77"/>
+      <c r="D219" s="77"/>
+      <c r="E219" s="77"/>
+      <c r="F219" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="G219" s="47" t="s">
+      <c r="G219" s="44" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="93" customHeight="1">
-      <c r="A220" s="48" t="s">
+      <c r="A220" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="B220" s="83" t="s">
+      <c r="B220" s="78" t="s">
         <v>226</v>
       </c>
-      <c r="C220" s="84"/>
-      <c r="D220" s="84"/>
-      <c r="E220" s="84"/>
-      <c r="F220" s="49" t="s">
+      <c r="C220" s="79"/>
+      <c r="D220" s="79"/>
+      <c r="E220" s="79"/>
+      <c r="F220" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="G220" s="50" t="s">
+      <c r="G220" s="47" t="s">
         <v>59</v>
       </c>
     </row>
@@ -13348,12 +14481,12 @@
       <c r="A221" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="B221" s="85" t="s">
+      <c r="B221" s="80" t="s">
         <v>228</v>
       </c>
-      <c r="C221" s="86"/>
-      <c r="D221" s="86"/>
-      <c r="E221" s="87"/>
+      <c r="C221" s="81"/>
+      <c r="D221" s="81"/>
+      <c r="E221" s="82"/>
       <c r="F221" s="15" t="s">
         <v>59</v>
       </c>
@@ -13365,12 +14498,12 @@
       <c r="A222" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B222" s="85" t="s">
+      <c r="B222" s="80" t="s">
         <v>229</v>
       </c>
-      <c r="C222" s="86"/>
-      <c r="D222" s="86"/>
-      <c r="E222" s="87"/>
+      <c r="C222" s="81"/>
+      <c r="D222" s="81"/>
+      <c r="E222" s="82"/>
       <c r="F222" s="18" t="s">
         <v>59</v>
       </c>
@@ -13382,12 +14515,12 @@
       <c r="A223" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="B223" s="88" t="s">
+      <c r="B223" s="83" t="s">
         <v>231</v>
       </c>
-      <c r="C223" s="81"/>
-      <c r="D223" s="81"/>
-      <c r="E223" s="81"/>
+      <c r="C223" s="76"/>
+      <c r="D223" s="76"/>
+      <c r="E223" s="76"/>
       <c r="F223" s="21" t="s">
         <v>59</v>
       </c>
@@ -13396,269 +14529,269 @@
       </c>
     </row>
     <row r="224" spans="1:7">
-      <c r="C224" s="51"/>
-    </row>
-    <row r="226" spans="1:7" ht="15.75" thickBot="1">
+      <c r="C224" s="48"/>
+    </row>
+    <row r="226" spans="1:7" ht="15" thickBot="1">
       <c r="A226" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="15.75" thickBot="1">
+    <row r="227" spans="1:7" ht="15" thickBot="1">
       <c r="A227" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="B227" s="38" t="s">
+      <c r="B227" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C227" s="52" t="s">
+      <c r="C227" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="D227" s="53" t="s">
+      <c r="D227" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E227" s="53"/>
-      <c r="F227" s="54"/>
-      <c r="G227" s="40" t="s">
+      <c r="E227" s="50"/>
+      <c r="F227" s="10"/>
+      <c r="G227" s="38" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="55">
+      <c r="A228" s="51">
         <v>42682</v>
       </c>
-      <c r="B228" s="56">
+      <c r="B228" s="52">
         <v>1.04</v>
       </c>
       <c r="C228" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D228" s="76" t="s">
+      <c r="D228" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="E228" s="76"/>
-      <c r="F228" s="76"/>
-      <c r="G228" s="57"/>
+      <c r="E228" s="71"/>
+      <c r="F228" s="71"/>
+      <c r="G228" s="25"/>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="58">
+      <c r="A229" s="53">
         <v>42692</v>
       </c>
-      <c r="B229" s="59">
+      <c r="B229" s="54">
         <v>1.05</v>
       </c>
       <c r="C229" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D229" s="75" t="s">
+      <c r="D229" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="E229" s="75"/>
-      <c r="F229" s="75"/>
-      <c r="G229" s="41"/>
+      <c r="E229" s="70"/>
+      <c r="F229" s="70"/>
+      <c r="G229" s="39"/>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="58">
+      <c r="A230" s="53">
         <v>42955</v>
       </c>
-      <c r="B230" s="59">
+      <c r="B230" s="54">
         <v>1.06</v>
       </c>
       <c r="C230" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D230" s="75" t="s">
+      <c r="D230" s="70" t="s">
         <v>235</v>
       </c>
-      <c r="E230" s="75"/>
-      <c r="F230" s="75"/>
-      <c r="G230" s="41"/>
+      <c r="E230" s="70"/>
+      <c r="F230" s="70"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="58">
+      <c r="A231" s="53">
         <v>42991</v>
       </c>
-      <c r="B231" s="59">
+      <c r="B231" s="54">
         <v>1.07</v>
       </c>
       <c r="C231" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D231" s="75" t="s">
+      <c r="D231" s="70" t="s">
         <v>236</v>
       </c>
-      <c r="E231" s="75"/>
-      <c r="F231" s="75"/>
-      <c r="G231" s="41"/>
+      <c r="E231" s="70"/>
+      <c r="F231" s="70"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="58">
+      <c r="A232" s="53">
         <v>43026</v>
       </c>
-      <c r="B232" s="59">
+      <c r="B232" s="54">
         <v>1.08</v>
       </c>
       <c r="C232" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D232" s="75" t="s">
+      <c r="D232" s="70" t="s">
         <v>237</v>
       </c>
-      <c r="E232" s="75"/>
-      <c r="F232" s="75"/>
-      <c r="G232" s="41"/>
+      <c r="E232" s="70"/>
+      <c r="F232" s="70"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="58">
+      <c r="A233" s="53">
         <v>43069</v>
       </c>
-      <c r="B233" s="59">
+      <c r="B233" s="54">
         <v>1.0900000000000001</v>
       </c>
       <c r="C233" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D233" s="75" t="s">
+      <c r="D233" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="E233" s="75"/>
-      <c r="F233" s="75"/>
-      <c r="G233" s="41"/>
+      <c r="E233" s="70"/>
+      <c r="F233" s="70"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="60">
+      <c r="A234" s="55">
         <v>43248</v>
       </c>
-      <c r="B234" s="61">
+      <c r="B234" s="56">
         <v>1.1000000000000001</v>
       </c>
       <c r="C234" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D234" s="71" t="s">
+      <c r="D234" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="E234" s="72"/>
-      <c r="F234" s="73"/>
-      <c r="G234" s="43"/>
+      <c r="E234" s="67"/>
+      <c r="F234" s="68"/>
+      <c r="G234" s="40"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="60">
+      <c r="A235" s="55">
         <v>43339</v>
       </c>
-      <c r="B235" s="61">
+      <c r="B235" s="56">
         <v>1.1100000000000001</v>
       </c>
       <c r="C235" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D235" s="71" t="s">
+      <c r="D235" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="E235" s="72"/>
-      <c r="F235" s="73"/>
-      <c r="G235" s="43"/>
+      <c r="E235" s="67"/>
+      <c r="F235" s="68"/>
+      <c r="G235" s="40"/>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="60">
+      <c r="A236" s="55">
         <v>43542</v>
       </c>
-      <c r="B236" s="61">
+      <c r="B236" s="56">
         <v>1.1200000000000001</v>
       </c>
       <c r="C236" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D236" s="71" t="s">
+      <c r="D236" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="72"/>
-      <c r="F236" s="73"/>
-      <c r="G236" s="43"/>
+      <c r="E236" s="67"/>
+      <c r="F236" s="68"/>
+      <c r="G236" s="40"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="60">
+      <c r="A237" s="55">
         <v>43599</v>
       </c>
-      <c r="B237" s="61">
+      <c r="B237" s="56">
         <v>1.1299999999999999</v>
       </c>
       <c r="C237" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D237" s="62" t="s">
+      <c r="D237" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="E237" s="63"/>
-      <c r="F237" s="64"/>
-      <c r="G237" s="43"/>
+      <c r="E237" s="58"/>
+      <c r="F237" s="59"/>
+      <c r="G237" s="40"/>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="60">
+      <c r="A238" s="55">
         <v>43643</v>
       </c>
-      <c r="B238" s="61">
+      <c r="B238" s="56">
         <v>1.1399999999999999</v>
       </c>
       <c r="C238" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D238" s="62" t="s">
+      <c r="D238" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E238" s="63"/>
-      <c r="F238" s="64"/>
-      <c r="G238" s="43"/>
+      <c r="E238" s="58"/>
+      <c r="F238" s="59"/>
+      <c r="G238" s="40"/>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="60">
+      <c r="A239" s="55">
         <v>43894</v>
       </c>
-      <c r="B239" s="61">
+      <c r="B239" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="C239" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D239" s="62" t="s">
+      <c r="D239" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="E239" s="63"/>
-      <c r="F239" s="64"/>
-      <c r="G239" s="43"/>
+      <c r="E239" s="58"/>
+      <c r="F239" s="59"/>
+      <c r="G239" s="40"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="60">
+      <c r="A240" s="55">
         <v>44017</v>
       </c>
-      <c r="B240" s="61">
+      <c r="B240" s="56">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C240" s="42" t="s">
+      <c r="C240" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D240" s="62" t="s">
+      <c r="D240" s="57" t="s">
         <v>239</v>
       </c>
-      <c r="E240" s="63"/>
-      <c r="F240" s="64"/>
-      <c r="G240" s="43"/>
-    </row>
-    <row r="241" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A241" s="65">
+      <c r="E240" s="58"/>
+      <c r="F240" s="59"/>
+      <c r="G240" s="40"/>
+    </row>
+    <row r="241" spans="1:7" ht="15" thickBot="1">
+      <c r="A241" s="60">
         <v>44118</v>
       </c>
-      <c r="B241" s="66">
+      <c r="B241" s="61">
         <v>1.17</v>
       </c>
       <c r="C241" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D241" s="74" t="s">
+      <c r="D241" s="69" t="s">
         <v>251</v>
       </c>
-      <c r="E241" s="74"/>
-      <c r="F241" s="74"/>
-      <c r="G241" s="44"/>
+      <c r="E241" s="69"/>
+      <c r="F241" s="69"/>
+      <c r="G241" s="41"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -13734,12 +14867,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>